<commit_message>
fix: imgui key enter not recognised. fix: text input element resizable and flags etc. add: cworld created with config and options for modules, threads etc. refactor: example modules systems
</commit_message>
<xml_diff>
--- a/resources/engine.xlsx
+++ b/resources/engine.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bogda\Desktop\Engine\KingdomsAndEmpires\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CAD4B1-DB8A-4E56-A40E-B66350B4A533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC51DFD1-0274-4402-93FA-BF455898225B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="4275" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="64">
   <si>
     <t>Feature ID</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>High</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>0.1</t>
@@ -235,12 +232,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -255,8 +258,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B10:T35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +620,7 @@
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N10" t="s">
         <v>2</v>
@@ -641,38 +645,40 @@
       </c>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="H11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" t="s">
         <v>12</v>
       </c>
-      <c r="M11" t="s">
-        <v>13</v>
-      </c>
       <c r="N11" t="s">
+        <v>61</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
         <v>62</v>
-      </c>
-      <c r="O11">
-        <v>1</v>
-      </c>
-      <c r="P11" t="s">
-        <v>63</v>
       </c>
       <c r="Q11" t="s">
         <v>10</v>
@@ -681,70 +687,74 @@
         <v>11</v>
       </c>
       <c r="S11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="T11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" t="s">
+      <c r="G12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-      <c r="J12" t="s">
-        <v>19</v>
+      <c r="H12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="G13" t="s">
-        <v>26</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
-      </c>
-      <c r="J13" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -753,25 +763,25 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
         <v>20</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
       <c r="G15" t="s">
         <v>11</v>
       </c>
@@ -779,24 +789,24 @@
         <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
         <v>22</v>
-      </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>23</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -805,21 +815,21 @@
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
         <v>47</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>48</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
@@ -828,139 +838,139 @@
         <v>11</v>
       </c>
       <c r="J17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
         <v>44</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18" t="s">
-        <v>45</v>
       </c>
       <c r="G18" t="s">
         <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
         <v>49</v>
-      </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>50</v>
       </c>
       <c r="G19" t="s">
         <v>10</v>
       </c>
       <c r="H19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
         <v>24</v>
       </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>25</v>
-      </c>
       <c r="G23" t="s">
         <v>11</v>
       </c>
       <c r="H23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" t="s">
         <v>26</v>
       </c>
-      <c r="I23" t="s">
-        <v>27</v>
-      </c>
       <c r="J23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" t="s">
         <v>32</v>
       </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" t="s">
-        <v>33</v>
-      </c>
       <c r="G24" t="s">
         <v>11</v>
       </c>
       <c r="H24" t="s">
+        <v>25</v>
+      </c>
+      <c r="I24" t="s">
         <v>26</v>
       </c>
-      <c r="I24" t="s">
-        <v>27</v>
-      </c>
       <c r="J24" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" t="s">
         <v>34</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25" t="s">
-        <v>35</v>
-      </c>
       <c r="G25" t="s">
         <v>11</v>
       </c>
       <c r="H25" t="s">
+        <v>25</v>
+      </c>
+      <c r="I25" t="s">
         <v>26</v>
       </c>
-      <c r="I25" t="s">
-        <v>27</v>
-      </c>
       <c r="J25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -969,157 +979,157 @@
         <v>10</v>
       </c>
       <c r="H27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" t="s">
         <v>37</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>38</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28" t="s">
-        <v>39</v>
-      </c>
       <c r="G28" t="s">
         <v>11</v>
       </c>
       <c r="H28" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" t="s">
         <v>26</v>
       </c>
-      <c r="I28" t="s">
-        <v>27</v>
-      </c>
       <c r="J28" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="29" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" t="s">
+        <v>53</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
         <v>54</v>
       </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29" t="s">
-        <v>55</v>
-      </c>
       <c r="G29" t="s">
         <v>11</v>
       </c>
       <c r="H29" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" t="s">
         <v>26</v>
       </c>
-      <c r="I29" t="s">
-        <v>27</v>
-      </c>
       <c r="J29" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" t="s">
         <v>41</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
         <v>42</v>
       </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30" t="s">
-        <v>43</v>
-      </c>
       <c r="G30" t="s">
         <v>11</v>
       </c>
       <c r="H30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J30" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
         <v>51</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
         <v>52</v>
-      </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33" t="s">
-        <v>53</v>
       </c>
       <c r="G33" t="s">
         <v>10</v>
       </c>
       <c r="H33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
+        <v>55</v>
+      </c>
+      <c r="D34" t="s">
         <v>56</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
         <v>57</v>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34" t="s">
-        <v>58</v>
-      </c>
       <c r="G34" t="s">
         <v>11</v>
       </c>
       <c r="H34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
         <v>59</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
         <v>60</v>
       </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>61</v>
-      </c>
       <c r="G35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring: engine and projects structure. Engine configuration and main entry point
</commit_message>
<xml_diff>
--- a/resources/engine.xlsx
+++ b/resources/engine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bogda\Desktop\Engine\KingdomsAndEmpires\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC51DFD1-0274-4402-93FA-BF455898225B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E84A95-A7A9-4B94-AB07-9E818E40EA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="74">
   <si>
     <t>Feature ID</t>
   </si>
@@ -63,6 +63,9 @@
     <t>High</t>
   </si>
   <si>
+    <t>In Progress</t>
+  </si>
+  <si>
     <t>0.1</t>
   </si>
   <si>
@@ -217,6 +220,33 @@
   </si>
   <si>
     <t>Engine 0.1</t>
+  </si>
+  <si>
+    <t>Asset Versioning</t>
+  </si>
+  <si>
+    <t>Asset ought to have a version number, so that, when they are loaded outdated assets can be detected and updated according to a update_asset_to_version function callback. This way updated engine will make older assets forward compatible and usable</t>
+  </si>
+  <si>
+    <t>Asset Pipeline, Virtual File System</t>
+  </si>
+  <si>
+    <t>Entity Inspector</t>
+  </si>
+  <si>
+    <t>Inspect an entity. Add/Remove/Edit components and tags. Change name.</t>
+  </si>
+  <si>
+    <t>World Outliner</t>
+  </si>
+  <si>
+    <t>Asset Browser</t>
+  </si>
+  <si>
+    <t>Show current entities in world as hierarchy tree or layered for rendering. Create new ones and delete. Reparent entities.</t>
+  </si>
+  <si>
+    <t>Show assets and resources associated with current project and allow to edit them</t>
   </si>
 </sst>
 </file>
@@ -232,7 +262,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +272,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -258,9 +294,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,7 +617,7 @@
   <dimension ref="B10:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="M10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N10" t="s">
         <v>2</v>
@@ -647,10 +684,10 @@
     <row r="11" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -666,19 +703,19 @@
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O11">
         <v>1</v>
       </c>
       <c r="P11" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="Q11" t="s">
         <v>10</v>
@@ -687,25 +724,25 @@
         <v>11</v>
       </c>
       <c r="S11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="T11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>10</v>
@@ -715,46 +752,94 @@
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="M12" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>10</v>
+      </c>
+      <c r="R12" t="s">
+        <v>11</v>
+      </c>
+      <c r="S12" t="s">
+        <v>64</v>
+      </c>
+      <c r="T12" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="M13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" t="s">
+        <v>70</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>11</v>
+      </c>
+      <c r="R13" t="s">
+        <v>11</v>
+      </c>
+      <c r="S13" t="s">
+        <v>64</v>
+      </c>
+      <c r="T13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -763,24 +848,48 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J14" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="M14" t="s">
+        <v>13</v>
+      </c>
+      <c r="N14" t="s">
+        <v>71</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>11</v>
+      </c>
+      <c r="R14" t="s">
+        <v>11</v>
+      </c>
+      <c r="S14" t="s">
+        <v>64</v>
+      </c>
+      <c r="T14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -789,24 +898,24 @@
         <v>11</v>
       </c>
       <c r="I15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G16" t="s">
         <v>10</v>
@@ -815,162 +924,190 @@
         <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D17" t="s">
-        <v>46</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17" t="s">
-        <v>47</v>
-      </c>
-      <c r="G17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" t="s">
-        <v>11</v>
-      </c>
-      <c r="J17" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G18" t="s">
         <v>10</v>
       </c>
       <c r="H18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="G19" t="s">
         <v>10</v>
       </c>
       <c r="H19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20" t="s">
+        <v>67</v>
+      </c>
+      <c r="J20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
         <v>25</v>
       </c>
-      <c r="J19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" t="s">
-        <v>23</v>
-      </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23" t="s">
-        <v>24</v>
-      </c>
       <c r="G23" t="s">
         <v>11</v>
       </c>
       <c r="H23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G24" t="s">
         <v>11</v>
       </c>
       <c r="H24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G25" t="s">
         <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J25" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" t="s">
         <v>36</v>
-      </c>
-      <c r="D27" t="s">
-        <v>35</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -979,157 +1116,157 @@
         <v>10</v>
       </c>
       <c r="H27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I27" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>39</v>
       </c>
-      <c r="J27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28" t="s">
-        <v>38</v>
-      </c>
       <c r="G28" t="s">
         <v>11</v>
       </c>
       <c r="H28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I28" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J28" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G29" t="s">
         <v>11</v>
       </c>
       <c r="H29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I29" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J29" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
       </c>
       <c r="H30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D33" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G33" t="s">
         <v>10</v>
       </c>
       <c r="H33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J33" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D34" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E34">
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G34" t="s">
         <v>11</v>
       </c>
       <c r="H34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J34" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="H35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="J35" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add tree sitter integration and text editor from other project
</commit_message>
<xml_diff>
--- a/resources/engine.xlsx
+++ b/resources/engine.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bogda\Desktop\Engine\KingdomsAndEmpires\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E84A95-A7A9-4B94-AB07-9E818E40EA20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C791F269-C7F6-4EE0-8ACE-52F30F6C94CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="76">
   <si>
     <t>Feature ID</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>Show assets and resources associated with current project and allow to edit them</t>
+  </si>
+  <si>
+    <t>Struct Property Editor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ability to edit a RTTR reflected structure that is provided as a rttr::variant or rttr::instance, so that the structure can be used to automatically construct an ImGui "editor" and the values be set to the correct values </t>
   </si>
 </sst>
 </file>
@@ -617,7 +623,7 @@
   <dimension ref="B10:T35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+      <selection activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,6 +932,30 @@
       <c r="J16" t="s">
         <v>19</v>
       </c>
+      <c r="M16" t="s">
+        <v>13</v>
+      </c>
+      <c r="N16" t="s">
+        <v>74</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>11</v>
+      </c>
+      <c r="R16" t="s">
+        <v>26</v>
+      </c>
+      <c r="S16" t="s">
+        <v>64</v>
+      </c>
+      <c r="T16" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>

</xml_diff>